<commit_message>
excel export in form c
</commit_message>
<xml_diff>
--- a/mainadminhtml/img/esop/uploadedby-Vinita_approver_userid-2.xlsx
+++ b/mainadminhtml/img/esop/uploadedby-Vinita_approver_userid-2.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CBSLD6\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\VPPLN2\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4B238D3-26D8-46ED-A932-9B3B17D39B0B}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8355"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
   <si>
     <t>Employee Name</t>
   </si>
@@ -36,19 +35,25 @@
     <t>No. of Shares</t>
   </si>
   <si>
+    <t>Harshad Jadhav</t>
+  </si>
+  <si>
+    <t>vinita mali</t>
+  </si>
+  <si>
+    <t>12345fdfd</t>
+  </si>
+  <si>
     <t>Date of Allotment(DD-MM-YYYY)</t>
   </si>
   <si>
-    <t>Rohit Singh</t>
-  </si>
-  <si>
-    <t>FTEPS11111</t>
+    <t>Subuser</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -360,11 +365,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -387,21 +392,21 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" t="s">
-        <v>5</v>
+        <v>3</v>
+      </c>
+      <c r="B2">
+        <v>123456</v>
       </c>
       <c r="C2">
-        <v>250</v>
+        <v>100</v>
       </c>
       <c r="D2" s="1">
-        <v>43831</v>
+        <v>43937</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -412,10 +417,38 @@
         <v>5</v>
       </c>
       <c r="C3">
-        <v>250</v>
+        <v>110</v>
       </c>
       <c r="D3" s="1">
-        <v>43831</v>
+        <v>43937</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4">
+        <v>3213113113</v>
+      </c>
+      <c r="C4">
+        <v>50</v>
+      </c>
+      <c r="D4" s="1">
+        <v>43937</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5">
+        <v>1333333333</v>
+      </c>
+      <c r="C5">
+        <v>40</v>
+      </c>
+      <c r="D5" s="1">
+        <v>43937</v>
       </c>
     </row>
   </sheetData>

</xml_diff>